<commit_message>
mengupdate file laporan word
</commit_message>
<xml_diff>
--- a/excel solver.xlsx
+++ b/excel solver.xlsx
@@ -1,88 +1,123 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\TRO\TUGAS TRO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/437a18f4103cac57/Documents/Teknik_Riset_Operasional/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22E1346C-A3E8-4258-9EE8-D93666DC7D33}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{22E1346C-A3E8-4258-9EE8-D93666DC7D33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{37158916-9641-4329-B4C9-38283ECF572F}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{B67F1BFB-EE3D-4C72-807C-E3A7DD0DAEF4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{B67F1BFB-EE3D-4C72-807C-E3A7DD0DAEF4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2 (2)" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="solver_adj" localSheetId="0" hidden="1">Sheet1!$B$9:$F$11,Sheet1!$B$14:$D$14</definedName>
     <definedName name="solver_adj" localSheetId="1" hidden="1">Sheet2!$C$7:$E$8</definedName>
+    <definedName name="solver_adj" localSheetId="2" hidden="1">'Sheet2 (2)'!$C$7:$E$8</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="2" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_drv" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_drv" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_eng" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_lhs1" localSheetId="0" hidden="1">Sheet1!$B$12:$F$12</definedName>
     <definedName name="solver_lhs1" localSheetId="1" hidden="1">Sheet2!$C$9:$E$9</definedName>
+    <definedName name="solver_lhs1" localSheetId="2" hidden="1">'Sheet2 (2)'!$C$9:$E$9</definedName>
     <definedName name="solver_lhs2" localSheetId="0" hidden="1">Sheet1!$G$9:$G$11</definedName>
     <definedName name="solver_lhs2" localSheetId="1" hidden="1">Sheet2!$F$7:$F$8</definedName>
+    <definedName name="solver_lhs2" localSheetId="2" hidden="1">'Sheet2 (2)'!$F$7:$F$8</definedName>
     <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="1" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="2" hidden="1">30</definedName>
     <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="1" hidden="1">0.075</definedName>
+    <definedName name="solver_mrt" localSheetId="2" hidden="1">0.075</definedName>
     <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_nod" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_num" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_num" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_opt" localSheetId="0" hidden="1">Sheet1!$H$2</definedName>
     <definedName name="solver_opt" localSheetId="1" hidden="1">Sheet2!$D$12</definedName>
+    <definedName name="solver_opt" localSheetId="2" hidden="1">'Sheet2 (2)'!$D$12</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
+    <definedName name="solver_pre" localSheetId="2" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rbv" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rbv" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_rel1" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_rel1" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_rel2" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel2" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rel2" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rhs1" localSheetId="0" hidden="1">Sheet1!$B$5:$F$5</definedName>
     <definedName name="solver_rhs1" localSheetId="1" hidden="1">Sheet2!$C$10:$E$10</definedName>
+    <definedName name="solver_rhs1" localSheetId="2" hidden="1">'Sheet2 (2)'!$C$10:$E$10</definedName>
     <definedName name="solver_rhs2" localSheetId="0" hidden="1">Sheet1!$H$9:$H$11</definedName>
     <definedName name="solver_rhs2" localSheetId="1" hidden="1">Sheet2!$H$7:$H$8</definedName>
+    <definedName name="solver_rhs2" localSheetId="2" hidden="1">'Sheet2 (2)'!$H$7:$H$8</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_scl" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_scl" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_ssz" localSheetId="0" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="1" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="2" hidden="1">100</definedName>
     <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="1" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="1" hidden="1">0.01</definedName>
+    <definedName name="solver_tol" localSheetId="2" hidden="1">0.01</definedName>
     <definedName name="solver_typ" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_typ" localSheetId="1" hidden="1">2</definedName>
+    <definedName name="solver_typ" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="1" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="2" hidden="1">3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -92,7 +127,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -100,7 +138,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="32">
   <si>
     <t>Nilai / Label</t>
   </si>
@@ -1056,7 +1094,7 @@
   <dimension ref="B1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1246,4 +1284,213 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30A2F242-FE6E-44EB-8D9A-B498CDD36E55}">
+  <dimension ref="B1:H12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" ht="15.75" thickBot="1">
+      <c r="B1" s="22"/>
+      <c r="C1" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="2:8" ht="15.75" thickBot="1">
+      <c r="B2" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="22">
+        <v>7</v>
+      </c>
+      <c r="D2" s="22">
+        <v>5</v>
+      </c>
+      <c r="E2" s="22">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" ht="15.75" thickBot="1">
+      <c r="B3" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="22">
+        <v>8</v>
+      </c>
+      <c r="D3" s="22">
+        <v>6</v>
+      </c>
+      <c r="E3" s="22">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" ht="15.75" thickBot="1">
+      <c r="B4" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="22">
+        <v>100</v>
+      </c>
+      <c r="D4" s="22">
+        <v>120</v>
+      </c>
+      <c r="E4" s="22">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" ht="15.75" thickBot="1"/>
+    <row r="6" spans="2:8" ht="15.75" thickBot="1">
+      <c r="B6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" ht="15.75" thickBot="1">
+      <c r="B7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="4">
+        <v>100</v>
+      </c>
+      <c r="D7" s="4">
+        <v>50</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0</v>
+      </c>
+      <c r="F7" s="26">
+        <f>SUM(C7:E7)</f>
+        <v>150</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7" s="4">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" ht="15.75" thickBot="1">
+      <c r="B8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0</v>
+      </c>
+      <c r="D8" s="4">
+        <v>70</v>
+      </c>
+      <c r="E8" s="4">
+        <v>130</v>
+      </c>
+      <c r="F8" s="26">
+        <f>SUM(C8:E8)</f>
+        <v>200</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H8" s="4">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" ht="15.75" thickBot="1">
+      <c r="B9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="26">
+        <f>SUM(C7:C8)</f>
+        <v>100</v>
+      </c>
+      <c r="D9" s="26">
+        <f t="shared" ref="D9:E9" si="0">SUM(D7:D8)</f>
+        <v>120</v>
+      </c>
+      <c r="E9" s="26">
+        <f t="shared" si="0"/>
+        <v>130</v>
+      </c>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+    </row>
+    <row r="10" spans="2:8" ht="15.75" thickBot="1">
+      <c r="B10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="4">
+        <v>100</v>
+      </c>
+      <c r="D10" s="4">
+        <v>120</v>
+      </c>
+      <c r="E10" s="4">
+        <v>130</v>
+      </c>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+    </row>
+    <row r="11" spans="2:8" ht="15.75" thickBot="1"/>
+    <row r="12" spans="2:8" ht="30.75" thickBot="1">
+      <c r="B12" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="25">
+        <f>SUMPRODUCT($C$2:$E$3,$C$7:$E$8)</f>
+        <v>2150</v>
+      </c>
+      <c r="D12" s="27"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DE31176-6093-4861-B8E5-881FEA6547A0}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>